<commit_message>
update export excel bill
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/export/orders_detail.xlsx
+++ b/src/main/webapp/WEB-INF/export/orders_detail.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuhung/Desktop/k2_tech_store/src/main/webapp/WEB-INF/export/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vuhung/Desktop/k2_tech_store/target/online_store_web/WEB-INF/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A54BE4-4633-6A4C-BFFB-6C5CA41CEB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53C9F90-E6AF-A448-A3BB-F26E213C86ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="19820" xr2:uid="{35F1A4C2-A5A5-C343-A8E8-AE2232428836}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16560" windowHeight="21600" xr2:uid="{35F1A4C2-A5A5-C343-A8E8-AE2232428836}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>jx:each(items="item.</t>
         </r>
@@ -115,7 +114,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>ordersDetailDtoList</t>
+          <t>exportProductDetailDtoList</t>
         </r>
         <r>
           <rPr>
@@ -123,7 +122,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>", var="</t>
         </r>
@@ -135,7 +133,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>ordersDetailDto</t>
+          <t>productDto</t>
         </r>
         <r>
           <rPr>
@@ -143,19 +141,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>", lastCell="L15")</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">", lastCell="L15")
 </t>
         </r>
       </text>
@@ -173,15 +160,9 @@
     <t>Đơn vị cung cấp:</t>
   </si>
   <si>
-    <t>K2 Tech Store</t>
-  </si>
-  <si>
     <t>Mã đơn hàng:</t>
   </si>
   <si>
-    <t>${item.code}</t>
-  </si>
-  <si>
     <t>Tên khách hàng:</t>
   </si>
   <si>
@@ -194,12 +175,6 @@
     <t>${item.customerName}</t>
   </si>
   <si>
-    <t>${item.phone}</t>
-  </si>
-  <si>
-    <t>${item.address}</t>
-  </si>
-  <si>
     <t>Lưu ý: Quý khách vui lòng kiểm tra lại thông tin danh sách sản phẩm trước khi nhận hàng.</t>
   </si>
   <si>
@@ -221,21 +196,6 @@
     <t>DANH SÁCH SẢN PHẨM</t>
   </si>
   <si>
-    <t>${orderDetailDto.productDto.productName}</t>
-  </si>
-  <si>
-    <t>${orderDetailDto.productDto.price}</t>
-  </si>
-  <si>
-    <t>$orderDetailDto.productDto.discount</t>
-  </si>
-  <si>
-    <t>${orderDetailDto.quantity}</t>
-  </si>
-  <si>
-    <t>${(orderDetailDto.productDto.price - orderDetailDto.productDto.price*orderDetailDto.productDto.discount) * orderDetailDto.quantity}</t>
-  </si>
-  <si>
     <t>Tổng thành tiền:</t>
   </si>
   <si>
@@ -245,29 +205,56 @@
     <t>Phí vận chuyển:</t>
   </si>
   <si>
-    <t>${item.ordersDto.shipping}</t>
-  </si>
-  <si>
     <t>Tổng tiền thu:</t>
   </si>
   <si>
-    <t>${item.totalAmount}</t>
-  </si>
-  <si>
     <t>Khách hàng ký xác nhận</t>
   </si>
   <si>
     <t>Nhà cung cấp</t>
   </si>
   <si>
-    <t>Vũ Văn Hùng</t>
+    <t>${item.manufactureName}</t>
+  </si>
+  <si>
+    <t>${item.orderCode}</t>
+  </si>
+  <si>
+    <t>${item.customerPhone}</t>
+  </si>
+  <si>
+    <t>${item.customerAddress}</t>
+  </si>
+  <si>
+    <t>${productDto.productName}</t>
+  </si>
+  <si>
+    <t>${productDto.price}</t>
+  </si>
+  <si>
+    <t>${item.amountShipping}</t>
+  </si>
+  <si>
+    <t>${item.amountTotal}</t>
+  </si>
+  <si>
+    <t>${item.founder}</t>
+  </si>
+  <si>
+    <t>${productDto.discount}</t>
+  </si>
+  <si>
+    <t>${productDto.quantity}</t>
+  </si>
+  <si>
+    <t>${productDto.totalAmount}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +316,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -367,36 +360,38 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,36 +710,36 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:11" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -755,12 +750,12 @@
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -771,12 +766,12 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -787,12 +782,12 @@
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -803,12 +798,12 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -820,7 +815,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -834,7 +829,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -848,146 +843,171 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="11"/>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="7"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="B16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8" t="s">
+      <c r="B17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="H20" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="C20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="H20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C24" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="H24" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H21:J23"/>
@@ -998,31 +1018,6 @@
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C21:E23"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>